<commit_message>
WIP: photo quotation, sales confirmation, purchase order
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/photo_quotation_to_supplier_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/photo_quotation_to_supplier_template.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Lead Items" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -424,9 +424,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>441360</xdr:colOff>
+      <xdr:colOff>441000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>808920</xdr:rowOff>
+      <xdr:rowOff>808560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -440,7 +440,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="19080"/>
-          <a:ext cx="1217880" cy="1227960"/>
+          <a:ext cx="1217520" cy="1227600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,7 +466,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>

</xml_diff>